<commit_message>
added power bi manual
</commit_message>
<xml_diff>
--- a/outputs/raw/Customer_List.xlsx
+++ b/outputs/raw/Customer_List.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,175 +443,133 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CUSTOMER1</t>
+          <t>CUST_1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CUSTOMER10</t>
+          <t>CUST_10</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CUSTOMER11</t>
+          <t>CUST_11</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CUSTOMER12</t>
+          <t>CUST_12</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CUSTOMER13</t>
+          <t>CUST_13</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CUSTOMER14</t>
+          <t>CUST_14</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CUSTOMER15</t>
+          <t>CUST_15</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CUSTOMER16</t>
+          <t>CUST_16</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CUSTOMER17</t>
+          <t>CUST_17</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CUSTOMER18</t>
+          <t>CUST_18</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CUSTOMER19</t>
+          <t>CUST_19</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CUSTOMER2</t>
+          <t>CUST_2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CUSTOMER20</t>
+          <t>CUST_3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CUSTOMER21</t>
+          <t>CUST_4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CUSTOMER22</t>
+          <t>CUST_5</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CUSTOMER23</t>
+          <t>CUST_6</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CUSTOMER24</t>
+          <t>CUST_7</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CUSTOMER25</t>
+          <t>CUST_8</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CUSTOMER3</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CUSTOMER4</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CUSTOMER5</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>CUSTOMER6</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CUSTOMER7</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CUSTOMER8</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>CUSTOMER9</t>
+          <t>CUST_9</t>
         </is>
       </c>
     </row>

</xml_diff>